<commit_message>
RPA-11:Sjekk Aktiv Trekk tvangs grunnlag
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v3.0_sample.xlsx
+++ b/Vasklister/Excel/vaskeliste_v3.0_sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6004" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6006" uniqueCount="43">
   <si>
     <t>debitor_ident</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>_4_Message</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -482,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,6 +645,12 @@
       <c r="S2" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
fixed issue with static delay entering infinite loop when searching the case history
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v3.0_sample.xlsx
+++ b/Vasklister/Excel/vaskeliste_v3.0_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24000" windowHeight="11130"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="19200" windowHeight="11130"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6008" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5989" uniqueCount="30">
   <si>
     <t>debitor_ident</t>
   </si>
@@ -79,42 +79,6 @@
     <t/>
   </si>
   <si>
-    <t>13088334935</t>
-  </si>
-  <si>
-    <t>267794</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>7100</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>FJELLHAMAR</t>
-  </si>
-  <si>
-    <t>984661185</t>
-  </si>
-  <si>
-    <t>POSTEN NORGE AS</t>
-  </si>
-  <si>
-    <t>Lørenskogveien 50_x000D_</t>
-  </si>
-  <si>
-    <t>1470 LØRENSKOG_x000D_</t>
-  </si>
-  <si>
-    <t>8 333,33</t>
-  </si>
-  <si>
     <t>_4_beløp</t>
   </si>
   <si>
@@ -139,16 +103,7 @@
     <t>_4_Message</t>
   </si>
   <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
     <t>Kommune_Nr</t>
-  </si>
-  <si>
-    <t>11111</t>
   </si>
 </sst>
 </file>
@@ -492,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC300"/>
+  <dimension ref="A1:AC299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,8 +467,10 @@
     <col min="16" max="19" width="11.42578125" style="1"/>
     <col min="20" max="20" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.42578125" style="1"/>
-    <col min="22" max="22" width="12.85546875" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" style="1" customWidth="1"/>
+    <col min="23" max="24" width="11.42578125" style="1"/>
+    <col min="25" max="25" width="15.85546875" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -523,8 +480,8 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>43</v>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -578,90 +535,93 @@
         <v>17</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -4583,7 +4543,7 @@
       <c r="E66" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G66" s="1" t="s">
@@ -4592,7 +4552,7 @@
       <c r="H66" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I66" s="3" t="s">
+      <c r="I66" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J66" s="1" t="s">
@@ -19078,69 +19038,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T300" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U300" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>